<commit_message>
Completed with View Balance
</commit_message>
<xml_diff>
--- a/Data/Result/ResLeaveMuster.xlsx
+++ b/Data/Result/ResLeaveMuster.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
   <si>
     <t>TestId</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1026,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>